<commit_message>
created Garret Specs txt file. Did Performance Evaluation on gradeChecker (CPU) on separte spreadsheet.
</commit_message>
<xml_diff>
--- a/Performance Metrics.xlsx
+++ b/Performance Metrics.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">AvgExecTime</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPI</t>
   </si>
   <si>
     <t xml:space="preserve">gradeChecker</t>
@@ -146,7 +149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -175,11 +178,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -232,7 +230,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -253,13 +251,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
@@ -286,170 +284,173 @@
       <c r="G1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>